<commit_message>
Added cvd ifr vs. vt turnover indicator. updated file paths with updated cvds
</commit_message>
<xml_diff>
--- a/outputs/BURs/tmp_Corporate.xlsx
+++ b/outputs/BURs/tmp_Corporate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">segment_function</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t xml:space="preserve">Q4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ytd_annualized</t>
   </si>
   <si>
     <t xml:space="preserve">Corporate</t>
@@ -527,16 +530,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -587,18 +593,21 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -649,16 +658,19 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -675,7 +687,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -687,16 +701,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -721,16 +738,17 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -783,6 +801,7 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -859,16 +878,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0.1171</v>
@@ -921,16 +943,19 @@
       <c r="T2" t="n">
         <v>0.0424</v>
       </c>
+      <c r="U2" t="n">
+        <v>0.2022</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -981,33 +1006,38 @@
       <c r="T3" t="n">
         <v>0.03816</v>
       </c>
+      <c r="U3" t="n">
+        <v>0.2022</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1171</v>
+        <v>0.0674</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0323</v>
+        <v>0.0133</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0417</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0314</v>
-      </c>
-      <c r="I4"/>
+        <v>0.0541</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0133</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -1019,16 +1049,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0.2022</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.333333333333333</v>
@@ -1071,16 +1104,17 @@
       <c r="T5" t="n">
         <v>0.5</v>
       </c>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -1133,16 +1167,17 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -1169,6 +1204,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1245,16 +1281,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -1305,18 +1344,21 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -1367,16 +1409,19 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -1393,7 +1438,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -1405,16 +1452,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.5</v>
@@ -1439,16 +1489,17 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -1501,6 +1552,7 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1577,19 +1629,22 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0955</v>
+        <v>0.0953</v>
       </c>
       <c r="E2" t="n">
         <v>0.0054</v>
@@ -1598,10 +1653,10 @@
         <v>0.0106</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0134</v>
+        <v>0.0133</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0295</v>
+        <v>0.0294</v>
       </c>
       <c r="I2" t="n">
         <v>0.0026</v>
@@ -1613,7 +1668,7 @@
         <v>0.0126</v>
       </c>
       <c r="L2" t="n">
-        <v>0.023</v>
+        <v>0.0229</v>
       </c>
       <c r="M2" t="n">
         <v>0.005</v>
@@ -1625,7 +1680,7 @@
         <v>0.0121</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0271</v>
+        <v>0.027</v>
       </c>
       <c r="Q2" t="n">
         <v>0.0096</v>
@@ -1639,16 +1694,19 @@
       <c r="T2" t="n">
         <v>0.0166</v>
       </c>
+      <c r="U2" t="n">
+        <v>0.1347</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -1658,10 +1716,10 @@
         <v>0.00954</v>
       </c>
       <c r="G3" t="n">
-        <v>0.01206</v>
+        <v>0.01197</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02655</v>
+        <v>0.02646</v>
       </c>
       <c r="I3" t="n">
         <v>0.00234</v>
@@ -1673,7 +1731,7 @@
         <v>0.01134</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0207</v>
+        <v>0.02061</v>
       </c>
       <c r="M3" t="n">
         <v>0.0045</v>
@@ -1685,7 +1743,7 @@
         <v>0.01089</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02439</v>
+        <v>0.0243</v>
       </c>
       <c r="Q3" t="n">
         <v>0.00864</v>
@@ -1699,33 +1757,38 @@
       <c r="T3" t="n">
         <v>0.01494</v>
       </c>
+      <c r="U3" t="n">
+        <v>0.1347</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0955</v>
+        <v>0.0449</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0054</v>
+        <v>0.0071</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0106</v>
+        <v>0.0047</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0134</v>
+        <v>0.007</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0295</v>
-      </c>
-      <c r="I4"/>
+        <v>0.0188</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0264</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -1737,16 +1800,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0.1347</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.5</v>
@@ -1797,16 +1863,17 @@
       <c r="T5" t="n">
         <v>0.4286</v>
       </c>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -1859,19 +1926,20 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.4</v>
+        <v>0.333333333333333</v>
       </c>
       <c r="E7" t="n">
         <v>0.5</v>
@@ -1885,7 +1953,9 @@
       <c r="H7" t="n">
         <v>0.4</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -1897,6 +1967,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1973,155 +2044,166 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1053</v>
+        <v>0.1038</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0127</v>
+        <v>0.0125</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0057</v>
+        <v>0.0056</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0102</v>
+        <v>0.0101</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0285</v>
+        <v>0.0281</v>
       </c>
       <c r="I2" t="n">
         <v>0.0044</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0076</v>
+        <v>0.0075</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0109</v>
+        <v>0.0107</v>
       </c>
       <c r="L2" t="n">
-        <v>0.023</v>
+        <v>0.0226</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0043</v>
+        <v>0.0042</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0118</v>
+        <v>0.0116</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0095</v>
+        <v>0.0093</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0256</v>
+        <v>0.0252</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0116</v>
+        <v>0.0114</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0073</v>
+        <v>0.0072</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0094</v>
+        <v>0.0092</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0283</v>
+        <v>0.0279</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1491</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.01143</v>
+        <v>0.01125</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00513</v>
+        <v>0.00504</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00918</v>
+        <v>0.00909</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02565</v>
+        <v>0.02529</v>
       </c>
       <c r="I3" t="n">
         <v>0.00396</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00684</v>
+        <v>0.00675</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00981</v>
+        <v>0.00963</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0207</v>
+        <v>0.02034</v>
       </c>
       <c r="M3" t="n">
-        <v>0.00387</v>
+        <v>0.00378</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01062</v>
+        <v>0.01044</v>
       </c>
       <c r="O3" t="n">
-        <v>0.00855</v>
+        <v>0.00837</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02304</v>
+        <v>0.02268</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.01044</v>
+        <v>0.01026</v>
       </c>
       <c r="R3" t="n">
-        <v>0.00657</v>
+        <v>0.00648</v>
       </c>
       <c r="S3" t="n">
-        <v>0.00846</v>
+        <v>0.00828</v>
       </c>
       <c r="T3" t="n">
-        <v>0.02547</v>
+        <v>0.02511</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.1491</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1053</v>
+        <v>0.0497</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0127</v>
+        <v>0.0051</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0057</v>
+        <v>0.0113</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0102</v>
+        <v>0.0156</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0285</v>
-      </c>
-      <c r="I4"/>
+        <v>0.032</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0178</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -2133,16 +2215,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0.1491</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.465909090909091</v>
@@ -2195,16 +2280,17 @@
       <c r="T5" t="n">
         <v>0.4</v>
       </c>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -2257,19 +2343,20 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5</v>
+        <v>0.461538461538462</v>
       </c>
       <c r="E7" t="n">
         <v>0.4286</v>
@@ -2283,7 +2370,9 @@
       <c r="H7" t="n">
         <v>0.5</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" t="n">
+        <v>0.4</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -2295,6 +2384,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2371,16 +2461,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2431,18 +2524,21 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -2493,17 +2589,20 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
@@ -2519,7 +2618,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -2531,16 +2632,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -2565,68 +2669,103 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="U6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2703,16 +2842,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2763,18 +2905,21 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -2825,16 +2970,19 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -2851,7 +2999,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -2863,6 +3013,9 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2939,16 +3092,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0.1205</v>
@@ -3001,16 +3157,19 @@
       <c r="T2" t="n">
         <v>0</v>
       </c>
+      <c r="U2" t="n">
+        <v>1.0344</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -3061,33 +3220,38 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>1.0344</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1205</v>
+        <v>0.3448</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.1667</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4"/>
+        <v>0.3333</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -3099,6 +3263,9 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>1.0344</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3175,16 +3342,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -3235,18 +3405,21 @@
         <v>0</v>
       </c>
       <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -3297,16 +3470,19 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
@@ -3323,7 +3499,9 @@
       <c r="H4" t="n">
         <v>0</v>
       </c>
-      <c r="I4"/>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -3335,6 +3513,9 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3411,155 +3592,166 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1116</v>
+        <v>0.1097</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0175</v>
+        <v>0.0173</v>
       </c>
       <c r="F2" t="n">
         <v>0.0035</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0105</v>
+        <v>0.0103</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0315</v>
+        <v>0.0311</v>
       </c>
       <c r="I2" t="n">
         <v>0.0034</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0068</v>
+        <v>0.0067</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0102</v>
+        <v>0.01</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0205</v>
+        <v>0.0201</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0134</v>
+        <v>0.0132</v>
       </c>
       <c r="O2" t="n">
-        <v>0.0099</v>
+        <v>0.0097</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0233</v>
+        <v>0.0229</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.0165</v>
+        <v>0.0162</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0066</v>
+        <v>0.0065</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0132</v>
+        <v>0.0129</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0362</v>
+        <v>0.0355</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.1179</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.01575</v>
+        <v>0.01557</v>
       </c>
       <c r="F3" t="n">
         <v>0.00315</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00945</v>
+        <v>0.00927</v>
       </c>
       <c r="H3" t="n">
-        <v>0.02835</v>
+        <v>0.02799</v>
       </c>
       <c r="I3" t="n">
         <v>0.00306</v>
       </c>
       <c r="J3" t="n">
-        <v>0.00612</v>
+        <v>0.00603</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00918</v>
+        <v>0.009</v>
       </c>
       <c r="L3" t="n">
-        <v>0.01845</v>
+        <v>0.01809</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0.01206</v>
+        <v>0.01188</v>
       </c>
       <c r="O3" t="n">
-        <v>0.00891</v>
+        <v>0.00873</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02097</v>
+        <v>0.02061</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.01485</v>
+        <v>0.01458</v>
       </c>
       <c r="R3" t="n">
-        <v>0.00594</v>
+        <v>0.00585</v>
       </c>
       <c r="S3" t="n">
-        <v>0.01188</v>
+        <v>0.01161</v>
       </c>
       <c r="T3" t="n">
-        <v>0.03258</v>
+        <v>0.03195</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.1179</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1116</v>
+        <v>0.0393</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0175</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0035</v>
+        <v>0.0163</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0105</v>
+        <v>0.0132</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0315</v>
-      </c>
-      <c r="I4"/>
+        <v>0.0294</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0099</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -3571,16 +3763,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0.1179</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.647058823529412</v>
@@ -3629,16 +3824,17 @@
       <c r="T5" t="n">
         <v>0.5</v>
       </c>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -3691,19 +3887,20 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -3713,7 +3910,9 @@
       <c r="H7" t="n">
         <v>0</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -3725,6 +3924,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3801,19 +4001,22 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2227</v>
+        <v>0.2188</v>
       </c>
       <c r="E2" t="n">
         <v>0.0217</v>
@@ -3828,51 +4031,54 @@
         <v>0.0438</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0227</v>
+        <v>0.0222</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0227</v>
+        <v>0.0222</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0451</v>
+        <v>0.0442</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0227</v>
+        <v>0.0222</v>
       </c>
       <c r="N2" t="n">
-        <v>0.0465</v>
+        <v>0.0455</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0.0682</v>
+        <v>0.0667</v>
       </c>
       <c r="Q2" t="n">
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0667</v>
+        <v>0.0652</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0656</v>
+        <v>0.0642</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.3846</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -3888,68 +4094,73 @@
         <v>0.03942</v>
       </c>
       <c r="I3" t="n">
-        <v>0.02043</v>
+        <v>0.01998</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.02043</v>
+        <v>0.01998</v>
       </c>
       <c r="L3" t="n">
-        <v>0.04059</v>
+        <v>0.03978</v>
       </c>
       <c r="M3" t="n">
-        <v>0.02043</v>
+        <v>0.01998</v>
       </c>
       <c r="N3" t="n">
-        <v>0.04185</v>
+        <v>0.04095</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.06138</v>
+        <v>0.06003</v>
       </c>
       <c r="Q3" t="n">
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.06003</v>
+        <v>0.05868</v>
       </c>
       <c r="S3" t="n">
         <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.05904</v>
+        <v>0.05778</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.3846</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2227</v>
+        <v>0.1282</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0217</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.0417</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0222</v>
+        <v>0.0444</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0438</v>
-      </c>
-      <c r="I4"/>
+        <v>0.0839</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.0455</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -3961,16 +4172,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0.3846</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.416666666666667</v>
@@ -4013,16 +4227,17 @@
       <c r="T5" t="n">
         <v>0.25</v>
       </c>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -4075,19 +4290,20 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.333333333333333</v>
+        <v>0.25</v>
       </c>
       <c r="E7" t="n">
         <v>0.3333</v>
@@ -4097,7 +4313,9 @@
       <c r="H7" t="n">
         <v>0.3333</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -4109,6 +4327,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4185,22 +4404,25 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1275</v>
+        <v>0.1131</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0196</v>
+        <v>0.0172</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -4209,19 +4431,19 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0195</v>
+        <v>0.0172</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0185</v>
+        <v>0.0164</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0172</v>
+        <v>0.0154</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0179</v>
+        <v>0.0159</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0536</v>
+        <v>0.0476</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -4239,28 +4461,31 @@
         <v>0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.0179</v>
+        <v>0.0159</v>
       </c>
       <c r="S2" t="n">
-        <v>0.0377</v>
+        <v>0.0333</v>
       </c>
       <c r="T2" t="n">
-        <v>0.0542</v>
+        <v>0.0482</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.0984</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
-        <v>0.01764</v>
+        <v>0.01548</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -4269,19 +4494,19 @@
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01755</v>
+        <v>0.01548</v>
       </c>
       <c r="I3" t="n">
-        <v>0.01665</v>
+        <v>0.01476</v>
       </c>
       <c r="J3" t="n">
-        <v>0.01548</v>
+        <v>0.01386</v>
       </c>
       <c r="K3" t="n">
-        <v>0.01611</v>
+        <v>0.01431</v>
       </c>
       <c r="L3" t="n">
-        <v>0.04824</v>
+        <v>0.04284</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
@@ -4299,41 +4524,46 @@
         <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.01611</v>
+        <v>0.01431</v>
       </c>
       <c r="S3" t="n">
-        <v>0.03393</v>
+        <v>0.02997</v>
       </c>
       <c r="T3" t="n">
-        <v>0.04878</v>
+        <v>0.04338</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.0984</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1275</v>
+        <v>0.0328</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0196</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0</v>
+        <v>0.0164</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.0167</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0195</v>
-      </c>
-      <c r="I4"/>
+        <v>0.0332</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -4345,16 +4575,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>0.0984</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0.142857142857143</v>
@@ -4391,16 +4624,17 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -4453,19 +4687,20 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
-        <v>0.5</v>
+        <v>0.285714285714286</v>
       </c>
       <c r="E7"/>
       <c r="F7" t="n">
@@ -4477,7 +4712,9 @@
       <c r="H7" t="n">
         <v>0.5</v>
       </c>
-      <c r="I7"/>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
@@ -4489,6 +4726,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4565,16 +4803,19 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -4626,17 +4867,20 @@
       </c>
       <c r="T2" t="n">
         <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1.7142</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3"/>
       <c r="E3" t="n">
@@ -4687,33 +4931,38 @@
       <c r="T3" t="n">
         <v>0</v>
       </c>
+      <c r="U3" t="n">
+        <v>1.7142</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>0.5714</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>0.3333</v>
       </c>
       <c r="H4" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4"/>
+        <v>0.5405</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4"/>
@@ -4725,16 +4974,19 @@
       <c r="R4"/>
       <c r="S4"/>
       <c r="T4"/>
+      <c r="U4" t="n">
+        <v>1.7142</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -4759,16 +5011,17 @@
       <c r="R5"/>
       <c r="S5"/>
       <c r="T5"/>
+      <c r="U5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="n">
         <v>0.5</v>
@@ -4821,16 +5074,17 @@
       <c r="T6" t="n">
         <v>0.5</v>
       </c>
+      <c r="U6"/>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -4855,6 +5109,7 @@
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
+      <c r="U7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>